<commit_message>
@push budg nouveau noyau
</commit_message>
<xml_diff>
--- a/0-docs/entreprenariat/Planning-TODO-LIST-INNOV-PROJECTs.xlsx
+++ b/0-docs/entreprenariat/Planning-TODO-LIST-INNOV-PROJECTs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="NOYAU" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
   <si>
     <t>Activité</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Permettre de genérer en lot tous les bulletins et les deposer dans un dossier indiquer par l'utilisateur</t>
+  </si>
+  <si>
+    <t>affichage des boutton sur pages en fonction du rôle utilisateur</t>
   </si>
 </sst>
 </file>
@@ -258,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,6 +329,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +903,7 @@
       <c r="E8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
@@ -1453,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1502,7 @@
       <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="32" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1507,7 +1513,7 @@
       <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="21" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1529,7 +1535,7 @@
       <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="21" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1540,7 +1546,7 @@
       <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="21" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1557,9 +1563,11 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
-        <v>43474</v>
-      </c>
-      <c r="B10" s="12"/>
+        <v>43496</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13">

</xml_diff>